<commit_message>
add new testscript files
</commit_message>
<xml_diff>
--- a/git/Automation test investigation .xlsx
+++ b/git/Automation test investigation .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RCVN\Desktop\git\php\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RCVN\Desktop\git-php\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E1DAD8-8779-46AA-9636-994FE1960470}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C2B4FB-6E7E-4763-96E7-3B7738CC81CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <author>RCVN</author>
   </authors>
   <commentList>
-    <comment ref="U21" authorId="0" shapeId="0" xr:uid="{ED41C54D-0DA0-4930-94CF-FA0957D944AC}">
+    <comment ref="U28" authorId="0" shapeId="0" xr:uid="{ED41C54D-0DA0-4930-94CF-FA0957D944AC}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
   <si>
     <t xml:space="preserve">1. The best automation test framework </t>
   </si>
@@ -318,6 +318,75 @@
   </si>
   <si>
     <t xml:space="preserve"> -&gt; need use latest xampp server. </t>
+  </si>
+  <si>
+    <t>https://github.com/alexandresalome/php-webdriver/blob/master/doc/cookies.rst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refer to selenenum page. </t>
+  </si>
+  <si>
+    <t>https://www.selenium.dev/documentation/en/support_packages/working_with_cookies/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">little about curl : </t>
+  </si>
+  <si>
+    <t>https://tutorialspoint.dev/language/php/php-curl</t>
+  </si>
+  <si>
+    <t>https://www.php.net/manual/en/book.curl.php</t>
+  </si>
+  <si>
+    <t>PHPNET</t>
+  </si>
+  <si>
+    <t>https://www.php.net/ArrayAccess</t>
+  </si>
+  <si>
+    <t>https://phpunit.readthedocs.io/en/9.3/textui.html#command-line-options</t>
+  </si>
+  <si>
+    <t>PHPUNIT</t>
+  </si>
+  <si>
+    <t>PHPDRIVER</t>
+  </si>
+  <si>
+    <t>SELENIUM DEV</t>
+  </si>
+  <si>
+    <t>https://github.com/xdebug/vscode-php-debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hướng dẫn install </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Kpib95hUlPQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">launch chrome using webdriver apis using curl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Details webdrives: </t>
+  </si>
+  <si>
+    <t>https://w3c.github.io/webdriver/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare chromedriver with curl </t>
+  </si>
+  <si>
+    <t>https://www.pawangaria.com/post/automation/browser-automation-from-command-line/</t>
+  </si>
+  <si>
+    <t>https://w3path.com/php-curl-what-is-curl-and-how-to-use-it/</t>
+  </si>
+  <si>
+    <t>Facebook\WebDriver\Exception\SessionNotCreatedException: Unable to create new service: ChromeDriverService</t>
+  </si>
+  <si>
+    <t>Lỗi ko start được chromeDriverService</t>
   </si>
 </sst>
 </file>
@@ -465,13 +534,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>170514</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>46689</xdr:colOff>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>75929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -509,13 +578,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>47087</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>9336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -815,345 +884,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B11A49-F9FD-4F4D-B685-AB1336E9C7D9}">
-  <dimension ref="B2:X72"/>
+  <dimension ref="B2:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:24">
       <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24">
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24">
+      <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24">
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:24">
-      <c r="B3">
+    <row r="10" spans="2:24">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
-      <c r="M4" t="s">
+    <row r="11" spans="2:24">
+      <c r="M11" t="s">
         <v>18</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T11" t="s">
         <v>28</v>
       </c>
-      <c r="U4" t="s">
+      <c r="U11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:24">
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:24">
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:24">
-      <c r="M7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-    </row>
-    <row r="8" spans="2:24">
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-    </row>
-    <row r="9" spans="2:24">
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-    </row>
-    <row r="10" spans="2:24">
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="T10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
     </row>
     <row r="12" spans="2:24">
       <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24">
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24">
+      <c r="M14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+    </row>
+    <row r="15" spans="2:24">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="T15" s="6"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+    </row>
+    <row r="16" spans="2:24">
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+    </row>
+    <row r="17" spans="2:24">
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+    </row>
+    <row r="19" spans="2:24">
+      <c r="B19">
         <v>3</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:24">
-      <c r="B14">
+    <row r="21" spans="2:24">
+      <c r="B21">
         <v>4</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C21" t="s">
         <v>63</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T21" t="s">
         <v>30</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:24">
-      <c r="C15" s="3" t="s">
+    <row r="22" spans="2:24">
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T22" t="s">
         <v>32</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:24">
-      <c r="C16" s="3" t="s">
+    <row r="23" spans="2:24">
+      <c r="C23" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:23">
-      <c r="C17" s="3" t="s">
+    <row r="24" spans="2:24">
+      <c r="C24" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:23">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:23">
-      <c r="C19" s="9" t="s">
+    <row r="25" spans="2:24">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="2:24">
+      <c r="C26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:23">
-      <c r="C20" s="3" t="s">
+    <row r="27" spans="2:24">
+      <c r="C27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="U20" t="s">
+      <c r="U27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:23">
-      <c r="C21" s="3"/>
-      <c r="U21" s="10" t="s">
+    <row r="28" spans="2:24">
+      <c r="C28" s="3"/>
+      <c r="U28" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="W28" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:23">
-      <c r="C22" s="3"/>
-      <c r="W22" s="3" t="s">
+    <row r="29" spans="2:24">
+      <c r="C29" s="3"/>
+      <c r="W29" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:23">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="2:23">
-      <c r="C24" s="3"/>
-    </row>
-    <row r="27" spans="2:23">
-      <c r="B27" t="s">
+    <row r="30" spans="2:24">
+      <c r="C30" s="3"/>
+      <c r="W30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="2:24">
+      <c r="C31" s="3"/>
+      <c r="W31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23">
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="2:23">
-      <c r="C28" t="s">
+    <row r="35" spans="2:23">
+      <c r="C35" t="s">
         <v>40</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:23">
-      <c r="C29" t="s">
+    <row r="36" spans="2:23">
+      <c r="C36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:23">
-      <c r="C31" t="s">
+    <row r="38" spans="2:23">
+      <c r="C38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="2:23">
-      <c r="C32" t="s">
+    <row r="39" spans="2:23">
+      <c r="C39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="3:3">
-      <c r="C48" t="s">
+    <row r="45" spans="2:23">
+      <c r="T45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="2:23">
+      <c r="W46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="3:23">
+      <c r="T49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="3:23">
+      <c r="W50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="3:23">
+      <c r="W51" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="3:23">
+      <c r="U53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="3:23">
+      <c r="W54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="3:23">
+      <c r="C55" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="3:11">
-      <c r="D49" t="s">
+      <c r="W55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="3:23">
+      <c r="D56" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="3:11">
-      <c r="D50" t="s">
+    <row r="57" spans="3:23">
+      <c r="D57" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="3:11">
-      <c r="C52" t="s">
+    <row r="59" spans="3:23">
+      <c r="C59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="3:11">
-      <c r="D53" t="s">
+    <row r="60" spans="3:23">
+      <c r="D60" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="3:11">
-      <c r="C55" t="s">
+    <row r="62" spans="3:23">
+      <c r="C62" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="3:11">
-      <c r="D56" s="8" t="s">
+    <row r="63" spans="3:23">
+      <c r="D63" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="3:11">
-      <c r="D57" t="s">
+    <row r="64" spans="3:23">
+      <c r="D64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="3:11">
-      <c r="C59" t="s">
+    <row r="66" spans="3:11">
+      <c r="C66" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="3:11">
-      <c r="D60" t="s">
+    <row r="67" spans="3:11">
+      <c r="D67" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="3:11">
-      <c r="D61" t="s">
+    <row r="68" spans="3:11">
+      <c r="D68" t="s">
         <v>60</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F68" t="s">
         <v>61</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K68" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="3:11">
-      <c r="D62" t="s">
+    <row r="69" spans="3:11">
+      <c r="D69" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="3:4">
-      <c r="C65" t="s">
+    <row r="72" spans="3:11">
+      <c r="C72" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="3:4">
-      <c r="C66" t="s">
+    <row r="73" spans="3:11">
+      <c r="C73" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="67" spans="3:4">
-      <c r="C67" t="s">
+    <row r="74" spans="3:11">
+      <c r="C74" t="s">
         <v>81</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D74" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="3:4">
-      <c r="C68" t="s">
+    <row r="75" spans="3:11">
+      <c r="C75" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="3:4">
-      <c r="C71" t="s">
+    <row r="78" spans="3:11">
+      <c r="C78" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="3:4">
-      <c r="C72" s="3" t="s">
+    <row r="79" spans="3:11">
+      <c r="C79" s="3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1" xr:uid="{57918199-1711-4372-8FFE-27EE7683AB7C}"/>
-    <hyperlink ref="U5" r:id="rId2" location="composer" xr:uid="{C2110FCC-AB6C-454D-BBF6-2D46390BDFA4}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{A8F91024-5662-4E2F-B304-48F29ACE08FE}"/>
-    <hyperlink ref="C15" r:id="rId4" xr:uid="{F6CBF3E9-1C9A-46F5-A5E0-2BE80B3FA680}"/>
-    <hyperlink ref="C16" r:id="rId5" xr:uid="{13A1C309-449A-4D7C-AAAC-4583F7FECEDD}"/>
-    <hyperlink ref="C17" r:id="rId6" location="new-session" xr:uid="{97C79A59-8502-4E3A-8F11-1831B2130F10}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{45D39740-4FE3-4CA6-A686-C58ED04FCF3A}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{968B1B0F-AA00-42D9-9D2E-A153CF66EE46}"/>
-    <hyperlink ref="W22" r:id="rId9" xr:uid="{ED6A6B7F-2EAA-4A6D-9AA2-A80EF994E271}"/>
-    <hyperlink ref="C72" r:id="rId10" xr:uid="{16667ED9-7B49-4ACD-8BC5-51C2EF814254}"/>
+    <hyperlink ref="M14" r:id="rId1" xr:uid="{57918199-1711-4372-8FFE-27EE7683AB7C}"/>
+    <hyperlink ref="U12" r:id="rId2" location="composer" xr:uid="{C2110FCC-AB6C-454D-BBF6-2D46390BDFA4}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{A8F91024-5662-4E2F-B304-48F29ACE08FE}"/>
+    <hyperlink ref="C22" r:id="rId4" xr:uid="{F6CBF3E9-1C9A-46F5-A5E0-2BE80B3FA680}"/>
+    <hyperlink ref="C23" r:id="rId5" xr:uid="{13A1C309-449A-4D7C-AAAC-4583F7FECEDD}"/>
+    <hyperlink ref="C24" r:id="rId6" location="new-session" xr:uid="{97C79A59-8502-4E3A-8F11-1831B2130F10}"/>
+    <hyperlink ref="C13" r:id="rId7" xr:uid="{45D39740-4FE3-4CA6-A686-C58ED04FCF3A}"/>
+    <hyperlink ref="C19" r:id="rId8" xr:uid="{968B1B0F-AA00-42D9-9D2E-A153CF66EE46}"/>
+    <hyperlink ref="W29" r:id="rId9" xr:uid="{ED6A6B7F-2EAA-4A6D-9AA2-A80EF994E271}"/>
+    <hyperlink ref="C79" r:id="rId10" xr:uid="{16667ED9-7B49-4ACD-8BC5-51C2EF814254}"/>
+    <hyperlink ref="W51" r:id="rId11" xr:uid="{57B45914-A9EE-4B42-B828-DDCF677D867E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
-  <drawing r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+  <drawing r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -1161,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1556,7 +1724,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC849BA3-B5DA-4611-AC38-8F50110DE0DA}">
-  <dimension ref="D7:I8"/>
+  <dimension ref="D7:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1577,6 +1745,16 @@
         <v>52</v>
       </c>
     </row>
+    <row r="10" spans="4:9">
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9">
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>